<commit_message>
update gsr indiv results
</commit_message>
<xml_diff>
--- a/derivatives/hyp_2-2_main-effect_exploratory_indiv/social/data_social-right.xlsx
+++ b/derivatives/hyp_2-2_main-effect_exploratory_indiv/social/data_social-right.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-eyeballs/derivatives/hyp_2-2_main-effect_exploratory_indiv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-eyeballs/derivatives/hyp_2-2_main-effect_exploratory_indiv/social/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE7B25C5-EFC6-7E46-A740-C93F6BD131B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E0E2C17-CD89-3C42-B3F1-D648ECEBB8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15100" xr2:uid="{7CDA5C90-3B20-C24C-974A-264C42CADE78}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16100" xr2:uid="{A8436BCA-643B-4D46-BC13-C0ABDA5FAD86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -66,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,2256 +385,2256 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFF54C8-04A2-8842-AB2E-FA911D4AA054}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326B0946-23AA-1C43-A80C-17D43556E6DE}">
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N51"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>-0.30497092420101962</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>-0.13448417734062745</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>-4.9713927306470576E-2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>6.7189478251862722E-2</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>-6.8181367518039215E-2</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>-0.12540536250201961</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>2.7391967668607839E-2</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>-0.10490467763686276</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>-5.1530550445686274E-2</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>0.25786860858294119</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>-0.31249919044337254</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="1">
         <v>0.13406446616931372</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="1">
         <v>3.8117030895490206E-2</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="1">
         <v>0.33742610039588233</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>-6.6640684301019618E-2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>-0.31360063424062745</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>-0.3388469751064706</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>-1.0092781548137281E-2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0.33311012538196078</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>-0.1573485402020196</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>0.13013597379860783</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>6.233549731372301E-4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>-0.58851980514568636</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>-0.39350367341705883</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>-1.0328375177433726</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>-5.2730559740686272E-2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>0.25228165675549019</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>5.7058185958823449E-3</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>0.1293639092989804</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1.3663198089372539E-2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.29236492429352945</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.41296971415186268</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.42693269788196075</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>3.5502624197980392E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>-0.12219428033139218</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>-1.656790036862775E-3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0.10017701322431373</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>1.0432938228829411</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>0.39127339605662748</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>0.52598354345931375</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>-0.36264532364450974</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>0.39348340529588233</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>-0.3536543758010196</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>-0.5800073066406275</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>-0.37162508760647062</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>-0.17055781554813729</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>-0.2057265998180392</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>-0.51163576320201964</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>-0.94382870163139221</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>-0.4262103540368628</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>3.3882275094313727E-2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>-0.50123849791705877</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
         <v>-0.90379736474337258</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>9.9843676119313732E-2</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <v>0.31900539945549022</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <v>0.38168802589588235</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>0.5946538794989803</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.55081850935937249</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.38712105589352941</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>0.6303825632518627</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.31815769188196075</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>0.17227115910798038</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>-0.13285752893139213</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>-0.22556126213686276</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>0.6382445138543138</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>0.1850883524829412</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
         <v>0.75278796545662752</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>0.52849186585931374</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>5.1212138195490212E-2</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>1.0699341739958823</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>-0.52929761630101968</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>-0.4053510628406275</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>-0.3461053865064706</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.22608727446186272</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>-5.8961668518039217E-2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>-0.38391009840201962</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>9.4459453458607845E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>-0.31010099623686277</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>-0.15897940454568626</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>-0.33143576861705881</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>0.24740658085662748</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>0.34378949935931374</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <v>0.39339070645549024</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>-9.2633082204117645E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>-0.48850539560101958</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>-0.64069896244062752</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>-0.73684440930647055</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>-0.27009741204813731</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>-0.63770449081803915</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>-1.0676568672020195</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>-0.48940099773139212</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>-0.37863254693686277</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>-0.50912266864568623</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>-1.9029803421170588</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>-0.85622823824337246</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>-0.35557679044068624</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="1">
         <v>-0.47551156704450981</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <v>-0.78470191110411769</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>0.26898371339898042</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>-0.12409135374062746</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0.38001862209352943</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>4.1586236851862718E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0.41745749358196077</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>0.14791457231098037</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>-0.60914982783139215</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>-0.97915865563686277</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>0.44520953735431373</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>-0.77080806971705873</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>0.68752532805662747</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>-0.15672716874068629</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <v>1.0507295882554901</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>0.39345100799588234</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>-0.25518236360101959</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>-0.57623120314062748</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>-9.0174585406470567E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>0.24624535174186274</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>0.2809810268819608</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>0.4105443593979804</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>-0.55892818893139218</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>-0.75917472293686283</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>1.8103812974313724E-2</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>0.1388865294829412</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>1.480162238662748E-2</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>-0.51187396744068625</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>-0.51422824234450981</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>0.88270109939588237</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>1.1566470098039062E-4</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.54721796245937249</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>0.25188389129352945</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>0.16354905270686271</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>1.0693799026819608</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>0.33549205649798042</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>-0.34061908353139214</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>-0.54565974373686277</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>0.65085643115431369</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>-0.6801482325170588</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="1">
         <v>0.26053596975662752</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>0.50668174645931374</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>0.29086495455549022</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <v>0.29874899799588234</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>-8.8782954471019609E-2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>-0.40389737934062742</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>-0.44210653890647056</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>0.39402012075186271</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>0.5503174773819608</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>0.32841584939798041</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>9.0897555686078324E-3</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>-3.9686305716862776E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>0.35217136895431372</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>0.39171381098294117</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>-0.68339247834337247</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>0.2673951005293137</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>-5.3584098544509795E-2</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>-0.38464144560411762</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>0.9287921674989803</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.9125123529593725</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>0.89266109539352945</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>0.43269180535186269</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>0.98140401668196087</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>0.82495099789798043</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>0.83223354256860782</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>0.88458915626313717</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>1.2709334785543138</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>0.58477147328294121</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="1">
         <v>0.53445518675662751</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>1.8541692622593138</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="1">
         <v>1.9814724183554902</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <v>2.4078610374958824</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>0.35961271019898039</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.31449649875937258</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>0.38227228329352941</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>0.19765654682186273</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>0.41949446998196077</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>0.16201645254798039</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>-0.50947057523139216</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>-0.14674621053686276</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>0.39429395645431375</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>-0.54335922121705871</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="1">
         <v>0.15280326779662748</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>1.0365045792593137</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="1">
         <v>3.8393703355490208E-2</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="1">
         <v>0.48548079519588233</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>-0.55062550010101963</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>-0.65421567074062748</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>-0.75081452560647055</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>-0.42597098864813721</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>-0.3293301672180392</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>-3.5520626020196233E-3</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>0.59719182026860784</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>-0.30592217503686281</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>-1.1443107744456862</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>0.65623056058294127</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="1">
         <v>-1.3216723577433724</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>-1.0576898977406861</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>-0.95337695564450975</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>-0.90813420150411772</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>-0.3732812757010196</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>-0.61756859794062746</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>-0.48327546440647062</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>-0.69747876194813729</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>-0.14468108781803923</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>-0.73927386410201956</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>-0.87738574263139224</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>-0.69112464743686275</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="1">
         <v>0.31794557215431374</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="1">
         <v>-1.1174219531170588</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="1">
         <v>-0.26293183234337253</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="1">
         <v>-0.78197157374068627</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="1">
         <v>-0.5488277179445098</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="1">
         <v>-0.58898455450411769</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>-0.24754919040101961</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>-0.42897554744062749</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>-0.69271357780647058</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>-0.63116589844813731</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>3.3867359981960776E-2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>-0.42585175780201956</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>-0.82178133203139214</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>-0.84893499423686281</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <v>-0.48941561574568632</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
         <v>-1.6623570591170587</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="1">
         <v>-0.82896196204337247</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>-0.38794651074068631</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="1">
         <v>0.50970122655549022</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="1">
         <v>-1.5445725195041176</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>-0.1834513861010196</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>-0.3734075738406275</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>-0.27426051560647058</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>-9.4001044648137272E-2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>0.23836955191196077</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>8.4185944607980387E-2</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>-5.5470223531392165E-2</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>2.1306013383137229E-2</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>-1.0810510704456862</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>3.2231902482941194E-2</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="1">
         <v>0.16737845600662749</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="1">
         <v>0.16737493515931373</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="1">
         <v>-0.37873028264450981</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="1">
         <v>-1.3576030415041176</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>-0.15736672900101961</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>-0.53337438434062745</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>-0.33388934550647059</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0.86335907375186272</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>1.0639050020819607</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>0.92383760759798039</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>0.21103830120860784</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>0.35457114436313719</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>0.35141694195431372</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <v>-0.10559614131705883</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="1">
         <v>-0.6154588671433725</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="1">
         <v>-0.30545582464068621</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="1">
         <v>-0.10618521394450978</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="1">
         <v>-0.86788384750411762</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>0.2150735378989804</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.25349407505937255</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>5.7304776023529423E-2</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>-6.5934346481372752E-3</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>0.4780130410819608</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>0.76004493979798038</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>0.52524930636860789</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>-0.15718353293686277</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <v>-0.29091849134568626</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="1">
         <v>0.1084480235629412</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="1">
         <v>7.6034960466274809E-3</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>-3.5472992540686255E-2</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="1">
         <v>-0.32683036684450983</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="1">
         <v>-0.10110789430411765</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>0.7041148735989804</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.37209526125937253</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>0.3680980344935294</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0.72000990055186276</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>0.77233644808196078</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>0.94703160989798041</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>0.49511887166860785</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <v>0.97271339356313724</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="1">
         <v>0.41933921715431371</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="1">
         <v>0.91638505668294123</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="1">
         <v>8.9400080106627478E-2</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>0.46280721525931379</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="1">
         <v>0.64873898075549019</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="1">
         <v>-3.7916103804117668E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>-0.10179896292101961</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>-0.24991429954062747</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>-8.3943121406470575E-2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>0.19279877797186273</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>-0.17066773461803925</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>0.11162179313798039</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>0.13915881438960784</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>2.0342098913137228E-2</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="1">
         <v>-0.16027289254568627</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="1">
         <v>-0.11911928981705883</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="1">
         <v>0.17339475681662747</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1">
         <v>-0.12874068474068626</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="1">
         <v>1.4518074755490218E-2</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="1">
         <v>-0.5365036365041177</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>-8.3845916801019618E-2</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.51667176205937249</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>0.54901272239352938</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>-0.2795734463481373</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>-2.7374754818039221E-2</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0.27605661879798038</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>0.21108714579860782</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>9.8176872793137221E-2</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>-2.2749159345686276E-2</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
         <v>-0.52527317041705879</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="1">
         <v>0.53091740295662748</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>0.22447960405931372</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="1">
         <v>-0.26213069514450982</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="1">
         <v>-0.21171336430411769</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>2.5117035468980392E-2</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>5.6808674929372541E-2</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.31481381399352942</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>0.29901166435186272</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>0.31901672848196078</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.35946193039798036</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>0.39413482616860784</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <v>0.15129811065313722</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <v>0.24247087115431373</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
         <v>1.0534415468829412</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="1">
         <v>0.53936837295662743</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1">
         <v>-0.12165895454068629</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="1">
         <v>-0.10901590244450979</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="1">
         <v>-7.3995764504117656E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>0.10905876399898039</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>2.1652730549372542E-2</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>-0.3923893825064706</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>-0.39462212054813728</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>-0.5535233821180392</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>-0.43620689710201965</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>0.20799496311860782</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="1">
         <v>-0.14175760373686278</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="1">
         <v>-0.35184407234568627</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="1">
         <v>-0.7818700261170588</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="1">
         <v>-0.18037181464337254</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <v>0.17589814564931372</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="1">
         <v>0.25393134455549021</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="1">
         <v>0.46799090459588233</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>-0.35571003130101958</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>-0.5653517388406275</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>-7.9299952006470567E-2</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>0.90315297385186277</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>0.78390388548196088</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>0.19377590718798038</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>-0.63284648983139213</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="1">
         <v>-8.0807041036862759E-2</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="1">
         <v>-5.6193697345686272E-2</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="1">
         <v>-0.76122453051705874</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="1">
         <v>-0.46753447274337256</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1">
         <v>0.64151207795931375</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="1">
         <v>0.33335410425549022</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="1">
         <v>-0.25887366150411767</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>0.65593861989898039</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0.43817333925937252</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>0.32754557449352945</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>-7.0911077848137272E-2</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>-0.76238029151803932</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>-0.16798794900201963</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>0.40990681736860785</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>0.96285911066313723</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <v>0.5804569535543137</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="1">
         <v>0.71018665948294124</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="1">
         <v>-0.59740199484337253</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>-0.71128384404068634</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="1">
         <v>-0.75625427284450975</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="1">
         <v>1.4977973124958823</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>0.35530142609898041</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>6.2937640979372544E-2</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>0.26640117569352945</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>0.28396088035186273</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>0.10583382535196077</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>-0.23775294120201962</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>3.6055481668607836E-2</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="1">
         <v>0.14158961287313723</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="1">
         <v>-0.11611430154568628</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="1">
         <v>0.79498425528294125</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="1">
         <v>0.75076328025662753</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1">
         <v>-0.67294737604068633</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="1">
         <v>0.2168478604554902</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="1">
         <v>0.28453305299588233</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>-0.53231957370101968</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>-0.35592688234062742</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>-0.12518105320647055</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>-0.76959356634813725</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>-1.0421694631180394</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>-0.27711494340201959</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>-0.19386027283139218</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>-7.1509217336862774E-2</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="1">
         <v>-0.41145204984568623</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="1">
         <v>-0.29825520991705884</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="1">
         <v>8.2651010466627484E-2</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="1">
         <v>-1.2981665407406862</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="1">
         <v>-1.1626057306445097</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="1">
         <v>4.9782549295882328E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>-0.30865704320101961</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0.24773549975937253</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>6.798863904352942E-2</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>0.43505666445186275</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>0.21912495209196076</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>-0.35875194420201961</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>-0.28723475343139215</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1">
         <v>-0.60772001283686283</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="1">
         <v>-8.4191374045686274E-2</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="1">
         <v>-6.3383393867058796E-2</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="1">
         <v>-0.18843299624337251</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="1">
         <v>-0.73916286544068632</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="1">
         <v>-0.99596046264450977</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="1">
         <v>9.9125633515882328E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>0.65685912179898032</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>1.5241186799593724</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>1.5280104843935296</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>0.84769158985186277</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>0.24921421277196076</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>0.6656737412979804</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>1.4236344203686078</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="1">
         <v>1.2227981633631373</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="1">
         <v>0.75509591315431379</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="1">
         <v>1.1372316608829411</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="1">
         <v>1.4817392372566276</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="1">
         <v>1.0740166107593137</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="1">
         <v>1.7557822773554903</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="1">
         <v>0.8938524282958823</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>0.53073413979898032</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>-0.19968747124062744</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>-0.18003231010647058</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>-5.8104417848137274E-2</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>-0.42394688331803926</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>0.34609351969798041</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>-0.26578412763139214</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1">
         <v>-0.26687149983686281</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="1">
         <v>-0.71199350334568634</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
         <v>-0.5731174296170588</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="1">
         <v>-0.65944619214337252</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1">
         <v>-0.14651186414068626</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="1">
         <v>-0.2131596213445098</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="1">
         <v>-1.0822109615041176</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>-0.25766786690101962</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>4.6809183759372541E-2</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>5.2758897153529424E-2</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>-0.10894772154813728</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>-9.3552102418039212E-2</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>-0.7681955022020196</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>-0.53925834363139213</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <v>-0.66579362543686282</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <v>0.21794656325431372</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="1">
         <v>-0.8381270314170588</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="1">
         <v>0.14393512854662749</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1">
         <v>0.12772923676931375</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="1">
         <v>0.83089835445549021</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="1">
         <v>0.47879620769588233</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>0.21970098559898041</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>0.75761893025937255</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>-1.654633106470571E-3</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>-0.32159493574813725</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>-0.27533807481803924</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>0.1836783165979804</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>0.12474960090860784</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>8.9512709793137232E-2</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="1">
         <v>-0.34181778394568629</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
         <v>0.2823548098829412</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="1">
         <v>0.41519769315662747</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="1">
         <v>0.13907121094931374</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="1">
         <v>-0.34443339974450982</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="1">
         <v>-0.71638617600411769</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>-0.25927522480101961</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>0.43869986905937253</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>0.47983555479352941</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>6.5587903051862712E-2</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>-5.4854024218039227E-2</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>-0.50089785090201966</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>-0.24357164343139215</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <v>-0.29273267363686278</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="1">
         <v>-3.402283694568628E-2</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="1">
         <v>0.4893607061829412</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="1">
         <v>-1.0189753433725163E-3</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="1">
         <v>0.18368328151431373</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="1">
         <v>-0.58549470804450976</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="1">
         <v>-0.41489266580411766</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>-0.26108661930101962</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>-0.14572170594062747</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>0.33510697449352944</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>0.76969125865186272</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>1.3068026838819606</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>0.81455624909798041</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>0.52644036406860784</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <v>0.4929447466631372</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="1">
         <v>0.83449782045431364</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="1">
         <v>1.0700553608829413</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="1">
         <v>0.12721036651662748</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="1">
         <v>0.87689381385931375</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="1">
         <v>6.3677578675490204E-2</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="1">
         <v>0.5831135823958824</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>0.79242385229898038</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>0.23785176205937253</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>-0.18203353210647061</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>7.2342725631862712E-2</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>-0.20272632261803925</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>-4.7670493502019601E-2</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>0.44247489746860785</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1">
         <v>0.77359467166313722</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="1">
         <v>-0.23211943794568629</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
         <v>0.96371696938294127</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="1">
         <v>-2.1867048743372502E-2</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="1">
         <v>0.32711031675931374</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="1">
         <v>0.19242964039549021</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="1">
         <v>-0.16803337710411764</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>-0.2153841856010196</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>0.34557561485937249</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>-0.40294823130647062</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>-0.44932601814813722</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>-0.28085725311803922</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>-0.29388410070201959</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <v>-0.66276672253139213</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="1">
         <v>-0.11535459143686277</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="1">
         <v>0.7202278491543137</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="1">
         <v>-0.17837800921705882</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="1">
         <v>0.39780501065662749</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="1">
         <v>6.2994932959313743E-2</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="1">
         <v>0.66383498295549026</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="1">
         <v>-0.18313273090411769</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>0.10482137409898039</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>0.23694547525937254</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>-4.412327570647058E-2</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>-1.2862932837481373</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>-0.89095037611803929</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>-0.48018805620201965</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <v>-7.8900368231392154E-2</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="1">
         <v>0.10995296138313723</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="1">
         <v>-0.18486461254568626</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="1">
         <v>-0.54936145811705872</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="1">
         <v>0.44452009005662746</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="1">
         <v>-9.8787902406862749E-3</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="1">
         <v>-0.61120766674450977</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="1">
         <v>-0.23630109190411769</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>-0.2882328445010196</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>5.7051038449372538E-2</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>0.3124851816935294</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>0.31226063235186274</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>-0.13634258091803925</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>0.24811842979798038</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <v>0.94783131516860786</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="1">
         <v>0.74746056186313725</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="1">
         <v>0.4827058264543137</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="1">
         <v>0.80383795408294123</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="1">
         <v>-0.1342529536433725</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="1">
         <v>-0.11270342094068628</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="1">
         <v>0.43239851195549017</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="1">
         <v>0.91475889739588234</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>0.52802138239898033</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>-0.15674596054062748</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>-0.2521969610064706</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>-0.56895686724813721</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>-0.76481866691803924</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>-0.65545998170201958</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <v>-0.14330315253139214</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="1">
         <v>1.2441172631372302E-3</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="1">
         <v>-0.3782270936456863</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="1">
         <v>0.23721940408294118</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="1">
         <v>-0.72291808674337255</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1">
         <v>-0.32139694384068629</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="1">
         <v>-0.26677821774450983</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="1">
         <v>-2.8405305804117681E-2</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>-0.13354819980101959</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>-0.4088387510406275</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>0.31362775119352942</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>-0.26475114964813729</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>-0.71171976551803917</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>-0.3585191619020196</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
         <v>-0.25966427563139216</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="1">
         <v>-6.5871782536862766E-2</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="1">
         <v>-0.35662197434568627</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="1">
         <v>-0.18584345561705881</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="1">
         <v>0.34463687125662745</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="1">
         <v>0.14925173896931374</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="1">
         <v>0.23068902665549021</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="1">
         <v>-0.56592225360411763</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>0.17779679199898041</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>0.47670685075937258</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>5.0660410393529427E-2</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>-2.6042800048137277E-2</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>0.19497881641196077</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>-0.20509475020201962</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <v>-0.19686140973139216</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="1">
         <v>-3.2783091368627712E-3</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="1">
         <v>0.51190574575431369</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="1">
         <v>0.56907298488294122</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="1">
         <v>0.11127617571862748</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="1">
         <v>-0.55823339814068629</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="1">
         <v>2.649676080549021E-2</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="1">
         <v>0.34075729029588231</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>-0.67390549560101964</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>-0.63034844914062749</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>-0.9570303186064707</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>-0.66135991754813728</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>-0.74515370761803923</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>-0.80091864760201958</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <v>-0.14088934063139213</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="1">
         <v>-0.12718564633686277</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="1">
         <v>-0.74947345694568623</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="1">
         <v>-0.11112402571705882</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="1">
         <v>-1.0672064877433725</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1">
         <v>-1.1593315647406861</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="1">
         <v>-1.2663844546445098</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="1">
         <v>-0.58880684910411762</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>-1.3354086866010195</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>-1.4429996670406275</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>-0.76992781380647057</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>-0.5009433516481373</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>-0.61240511841803924</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>-0.77259167160201958</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
         <v>-1.2009630876313921</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="1">
         <v>-1.1201692476368628</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="1">
         <v>-0.8330145613456863</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="1">
         <v>-2.0100161391170586</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="1">
         <v>-0.4407568848433725</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="1">
         <v>-0.90077846174068632</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="1">
         <v>-0.86818852924450973</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="1">
         <v>-0.94095858850411773</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>-9.3656974881019608E-2</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>-6.1056157740627448E-2</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>-0.23468829270647057</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>4.8983687151862715E-2</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <v>-0.1071456947180392</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>-0.21971372170201964</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="1">
         <v>-0.33940556643139214</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="1">
         <v>-0.2745751308368628</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="1">
         <v>-0.19995415004568629</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="1">
         <v>-0.25986227151705882</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="1">
         <v>-9.6759986433725131E-3</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="1">
         <v>-0.25696367574068624</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="1">
         <v>0.39764501925549023</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="1">
         <v>-6.1302747004117669E-2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>0.51936342049898032</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>0.77702915155937247</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>0.47850329259352942</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>-1.7325168848137285E-2</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <v>0.71740863518196085</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>0.34515135459798041</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="1">
         <v>0.63491316536860776</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="1">
         <v>0.38344454066313721</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="1">
         <v>0.21673142605431372</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="1">
         <v>0.75770130618294129</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="1">
         <v>1.1206287862566275</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="1">
         <v>0.76009113225931368</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="1">
         <v>0.86861991095549029</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="1">
         <v>0.97987746609588233</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>0.69773445739898032</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>0.84524963155937249</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>0.44530264149352938</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>-0.70074510594813721</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <v>-0.71346578241803926</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>0.15278745848798039</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="1">
         <v>0.21802650486860783</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="1">
         <v>0.2671689288631372</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="1">
         <v>0.21763668565431371</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="1">
         <v>-0.58792204751705879</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="1">
         <v>0.63518571395662748</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="1">
         <v>0.56667124395931379</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="1">
         <v>0.63282361505549023</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="1">
         <v>1.1296724260958824</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>-5.4542868051019607E-2</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>9.6839341063372539E-2</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>-0.20108353760647057</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>-0.22316174334813729</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="1">
         <v>-5.4696444318039217E-2</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>-8.4355542602019606E-2</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="1">
         <v>0.29046807706860783</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="1">
         <v>-7.9665936636862777E-2</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="1">
         <v>-0.11111535864568628</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="1">
         <v>-0.30541385461705883</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="1">
         <v>1.3769756426627477E-2</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="1">
         <v>-0.27659823604068623</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="1">
         <v>0.14555331703549021</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="1">
         <v>-0.20864154220411768</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>0.80043278589898037</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>0.22059301825937255</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>-0.3154497328064706</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>-8.4838440448137292E-2</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="1">
         <v>-1.3158619911180394</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>0.28352352619798038</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="1">
         <v>1.0799773468686078</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="1">
         <v>1.4380645553631373</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="1">
         <v>-0.23777487434568628</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="1">
         <v>2.8021805638829411</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="1">
         <v>-0.38157145884337251</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="1">
         <v>-0.22460326324068627</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="1">
         <v>-0.80740845624450974</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="1">
         <v>-0.85881481150411776</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>-0.37857884100101963</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>-0.45769076404062747</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>0.40229466699352939</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>0.31939430865186269</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="1">
         <v>0.11990983937196079</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>0.36044316139798038</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="1">
         <v>-2.7907192731392166E-2</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="1">
         <v>0.30770725006313721</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="1">
         <v>0.49382106745431376</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="1">
         <v>9.1497002294119167E-4</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="1">
         <v>0.25278250665662749</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="1">
         <v>-0.10630021394068626</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="1">
         <v>-9.0465908944509787E-2</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="1">
         <v>7.4270086185882336E-2</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>-0.4410868828010196</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>9.0819649127372545E-2</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
         <v>0.19628002348352941</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>0.14736908538186272</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="1">
         <v>-1.5384088018039227E-2</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <v>0.60678829179798033</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="1">
         <v>0.66554049596860787</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="1">
         <v>0.3919878582631372</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="1">
         <v>-0.37840526914568628</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="1">
         <v>0.16996300918294119</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="1">
         <v>0.81848166475662754</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="1">
         <v>0.15419614773931373</v>
       </c>
-      <c r="M51">
+      <c r="M51" s="1">
         <v>-0.57400038814450971</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="1">
         <v>-0.64773417030411762</v>
       </c>
     </row>

</xml_diff>